<commit_message>
minor updates to iterators
</commit_message>
<xml_diff>
--- a/tests/testdata.xlsx
+++ b/tests/testdata.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="96" windowWidth="28752" windowHeight="12588"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" calcOnSave="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -63,47 +63,47 @@
     <t>strin,"dfe\"ns</t>
   </si>
   <si>
+    <t>apostle</t>
+  </si>
+  <si>
+    <t>colors</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>ペトロ</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
     <t>"'bart',"dfe\"ns</t>
-  </si>
-  <si>
-    <t>apostle</t>
-  </si>
-  <si>
-    <t>colors</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>black</t>
-  </si>
-  <si>
-    <t>yellow</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>ペトロ</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,9 +132,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -249,6 +250,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -283,6 +285,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -458,24 +461,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" customWidth="1"/>
     <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -484,7 +489,7 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
         <v>12</v>
@@ -493,7 +498,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -504,7 +509,7 @@
         <v>0.82476099999999997</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -513,7 +518,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -524,7 +529,7 @@
         <v>0.56825400000000004</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -533,7 +538,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -544,7 +549,7 @@
         <v>0.66207400000000005</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>5</v>
@@ -553,7 +558,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -564,7 +569,7 @@
         <v>5.5173E-2</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>12</v>
@@ -573,7 +578,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -584,16 +589,16 @@
         <v>0.51263700000000001</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>6</v>
       </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -604,7 +609,7 @@
         <v>0.74686699999999995</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>9</v>
@@ -613,9 +618,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8">
         <v>0.46800000000000003</v>
@@ -624,7 +629,7 @@
         <v>0.60611000000000004</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -633,7 +638,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -644,7 +649,7 @@
         <v>0.58596899999999996</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -653,7 +658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -664,7 +669,7 @@
         <v>0.2392</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -673,7 +678,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -684,7 +689,7 @@
         <v>0.76299099999999997</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11">
         <v>11</v>
@@ -693,7 +698,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -704,7 +709,7 @@
         <v>0.66080499999999998</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -713,7 +718,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -724,7 +729,7 @@
         <v>7.5856999999999994E-2</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -743,27 +748,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -774,7 +779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
@@ -785,7 +790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7</v>
       </c>
@@ -805,12 +810,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>